<commit_message>
Color Coded Adjacency Test on Spreadsheet
</commit_message>
<xml_diff>
--- a/ClueGameBoardSpreadsheet.xlsx
+++ b/ClueGameBoardSpreadsheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhonathan's PC\Desktop\Software Engineering\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8375EF-771C-4A1F-9BAF-1FA216D2C717}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,16 +450,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y24" sqref="A1:Y24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -535,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -612,7 +613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -689,7 +690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -766,7 +767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -843,7 +844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -920,7 +921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -997,7 +998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1074,7 +1075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1228,7 +1229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1305,7 +1306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1382,7 +1383,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1536,7 +1537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1690,7 +1691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1767,7 +1768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1921,7 +1922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -2152,7 +2153,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>

</xml_diff>